<commit_message>
GL update - Item build report
- changed the template of exported file
- added as_of and period in custom filtering
</commit_message>
<xml_diff>
--- a/public/excel_templates/item-build-report-template.xlsx
+++ b/public/excel_templates/item-build-report-template.xlsx
@@ -21,14 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Out Qty</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58,21 +50,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -82,15 +65,17 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -372,18 +357,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="5" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" style="5"/>
-    <col min="6" max="6" width="9.140625" style="5" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="5"/>
+    <col min="1" max="1" width="11.42578125" style="4" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="9.140625" style="4" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -415,57 +400,33 @@
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
-      <c r="G3"/>
+      <c r="G3" s="7"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="I5" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="A6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>